<commit_message>
Adjustment Service Export Data Excel
</commit_message>
<xml_diff>
--- a/public/Storage/users.xlsx
+++ b/public/Storage/users.xlsx
@@ -11,27 +11,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
-  <si>
-    <t>Inisial Nama</t>
-  </si>
-  <si>
-    <t>Umur</t>
-  </si>
-  <si>
-    <t>Umur Kandungan</t>
-  </si>
-  <si>
-    <t>Pendidikan</t>
-  </si>
-  <si>
-    <t>Tingkat Pendapatan</t>
-  </si>
-  <si>
-    <t>Total Post-test</t>
-  </si>
-  <si>
-    <t>Total Pre-test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+  <si>
+    <t>Screening</t>
+  </si>
+  <si>
+    <t>Pretest</t>
+  </si>
+  <si>
+    <t>Posttest</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Question 5</t>
+  </si>
+  <si>
+    <t>Question 6</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Question 8</t>
+  </si>
+  <si>
+    <t>Question 9</t>
+  </si>
+  <si>
+    <t>Question 10</t>
+  </si>
+  <si>
+    <t>Question 11</t>
+  </si>
+  <si>
+    <t>Question 12</t>
+  </si>
+  <si>
+    <t>Question 13</t>
+  </si>
+  <si>
+    <t>Question 14</t>
   </si>
   <si>
     <t>Vivi</t>
@@ -62,6 +92,9 @@
   </si>
   <si>
     <t>ER</t>
+  </si>
+  <si>
+    <t>Putria</t>
   </si>
 </sst>
 </file>
@@ -442,179 +475,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:AK9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="12" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+    </row>
+    <row r="2" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="O2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="P2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
       <c r="F5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F6">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
         <v>14</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:W1"/>
+    <mergeCell ref="X1:AK1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>